<commit_message>
Update by Vaishnavi on Task 3.2
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Task ID 1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Task ID 3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Task ID 1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Task ID 3" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -198,13 +198,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -222,7 +222,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -253,13 +253,13 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -282,14 +282,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -317,8 +317,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -344,8 +344,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -371,13 +371,13 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -401,7 +401,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -429,8 +429,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -456,8 +456,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -483,7 +483,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -498,16 +498,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -528,16 +528,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -558,16 +558,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -578,7 +578,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>3</col>
@@ -593,9 +593,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -615,9 +615,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -637,9 +637,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -649,7 +649,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -664,16 +664,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -694,16 +694,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -724,16 +724,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -754,16 +754,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -784,16 +784,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -814,16 +814,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -844,16 +844,16 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -874,13 +874,41 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId8"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>138</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5715000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1479,6 +1507,16 @@
           <t>Vaishnavi</t>
         </is>
       </c>
+      <c r="F9" s="8" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2025-05-04 07:42:19</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1786,7 +1824,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -1817,7 +1855,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>44.44%</t>
+          <t>55.56%</t>
         </is>
       </c>
     </row>
@@ -1829,7 +1867,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.2</t>
         </is>
       </c>
     </row>
@@ -1853,7 +1891,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 11:33:17</t>
+          <t>2025-05-04 07:42:19</t>
         </is>
       </c>
     </row>
@@ -1865,7 +1903,7 @@
       </c>
       <c r="B12" s="10" t="inlineStr">
         <is>
-          <t>[███████████---------] 55%</t>
+          <t>[█████████████-------] 66%</t>
         </is>
       </c>
     </row>
@@ -1898,7 +1936,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1930,7 +1968,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1945,7 +1983,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B133"/>
+  <dimension ref="A1:B155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2133,6 +2171,7 @@
         </is>
       </c>
     </row>
+    <row r="112"/>
     <row r="113">
       <c r="A113" s="9" t="inlineStr">
         <is>
@@ -2182,6 +2221,20 @@
       </c>
     </row>
     <row r="117" ht="100" customHeight="1"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
     <row r="132">
       <c r="A132" s="9" t="inlineStr">
         <is>
@@ -2203,6 +2256,79 @@
       <c r="B133" s="9" t="inlineStr">
         <is>
           <t>tes</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="9" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B135" s="9" t="inlineStr">
+        <is>
+          <t>Task 3.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="9" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B136" s="9" t="inlineStr">
+        <is>
+          <t>Home &gt; Dashboard</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="9" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B137" s="9" t="inlineStr">
+        <is>
+          <t>Vaishnavi</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="9" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B138" s="9" t="inlineStr">
+        <is>
+          <t>2025-05-04 07:42:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="139" ht="100" customHeight="1"/>
+    <row r="154">
+      <c r="A154" s="9" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B154" s="11" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="9" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B155" s="9" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update by Yash on Task 2.0
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Task ID 1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Task ID 3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Task ID 2" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -407,12 +408,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Summary'!$A$40:$A$41</f>
+              <f>'Summary'!$A$40:$A$42</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Summary'!$B$40:$B$41</f>
+              <f>'Summary'!$B$40:$B$42</f>
             </numRef>
           </val>
         </ser>
@@ -909,6 +910,39 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="4552950" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1387,6 +1421,16 @@
           <t>Yash</t>
         </is>
       </c>
+      <c r="F5" s="8" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-05-04 07:50:25</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1796,7 +1840,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
@@ -1824,7 +1868,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -1855,7 +1899,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>55.56%</t>
+          <t>66.67%</t>
         </is>
       </c>
     </row>
@@ -1867,7 +1911,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>2.0</t>
         </is>
       </c>
     </row>
@@ -1879,7 +1923,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Vaishnavi</t>
+          <t>Yash</t>
         </is>
       </c>
     </row>
@@ -1891,7 +1935,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 07:42:19</t>
+          <t>2025-05-04 07:50:25</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1947,7 @@
       </c>
       <c r="B12" s="10" t="inlineStr">
         <is>
-          <t>[█████████████-------] 66%</t>
+          <t>[███████████████-----] 77%</t>
         </is>
       </c>
     </row>
@@ -1936,7 +1980,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1969,6 +2013,16 @@
       </c>
       <c r="B41" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Yash</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2043,110 +2097,12 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
     <row r="20" ht="100" customHeight="1"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
     <row r="35" ht="100" customHeight="1"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
     <row r="50" ht="100" customHeight="1"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
     <row r="65" ht="100" customHeight="1"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
     <row r="80" ht="100" customHeight="1"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
     <row r="95" ht="100" customHeight="1"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
@@ -2171,7 +2127,6 @@
         </is>
       </c>
     </row>
-    <row r="112"/>
     <row r="113">
       <c r="A113" s="9" t="inlineStr">
         <is>
@@ -2221,20 +2176,6 @@
       </c>
     </row>
     <row r="117" ht="100" customHeight="1"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
     <row r="132">
       <c r="A132" s="9" t="inlineStr">
         <is>
@@ -2327,6 +2268,102 @@
         </is>
       </c>
       <c r="B155" s="9" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>Task 2.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B2" s="9" t="inlineStr">
+        <is>
+          <t>Dashboard &gt; Settings &gt; Logout</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>Yash</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>2025-05-04 07:50:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="100" customHeight="1"/>
+    <row r="20">
+      <c r="A20" s="9" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B20" s="11" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="9" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B21" s="9" t="inlineStr">
         <is>
           <t>test</t>
         </is>

</xml_diff>

<commit_message>
Update by Yash on Task 2.1
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -943,6 +943,34 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>26</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1714500" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1456,6 +1484,16 @@
           <t>Yash</t>
         </is>
       </c>
+      <c r="F6" s="8" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-05-04 07:56:02</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1868,7 +1906,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -1899,7 +1937,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>66.67%</t>
+          <t>77.78%</t>
         </is>
       </c>
     </row>
@@ -1911,7 +1949,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2.1</t>
         </is>
       </c>
     </row>
@@ -1935,7 +1973,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 07:50:25</t>
+          <t>2025-05-04 07:56:02</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1985,7 @@
       </c>
       <c r="B12" s="10" t="inlineStr">
         <is>
-          <t>[███████████████-----] 77%</t>
+          <t>[█████████████████---] 88%</t>
         </is>
       </c>
     </row>
@@ -1980,7 +2018,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -2022,7 +2060,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2285,7 +2323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2345,6 +2383,20 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
     <row r="20">
       <c r="A20" s="9" t="inlineStr">
         <is>
@@ -2366,6 +2418,79 @@
       <c r="B21" s="9" t="inlineStr">
         <is>
           <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B23" s="9" t="inlineStr">
+        <is>
+          <t>Task 2.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="9" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B24" s="9" t="inlineStr">
+        <is>
+          <t>Dashboard &gt; Logout &gt; Button</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B25" s="9" t="inlineStr">
+        <is>
+          <t>Yash</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="9" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B26" s="9" t="inlineStr">
+        <is>
+          <t>2025-05-04 07:56:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="100" customHeight="1"/>
+    <row r="42">
+      <c r="A42" s="9" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B42" s="11" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="9" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B43" s="9" t="inlineStr">
+        <is>
+          <t>Anmol mobile</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update by Vaishnavi on Task 3.0
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Task ID 1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Task ID 3" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -35,7 +36,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -52,6 +53,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00ADD8E6"/>
         <bgColor rgb="00ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF6347"/>
+        <bgColor rgb="00FF6347"/>
       </patternFill>
     </fill>
   </fills>
@@ -82,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -94,6 +101,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,12 +389,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Summary'!$A$40</f>
+              <f>'Summary'!$A$40:$A$41</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Summary'!$B$40</f>
+              <f>'Summary'!$B$40:$B$41</f>
             </numRef>
           </val>
         </ser>
@@ -478,6 +487,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -551,6 +563,36 @@
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400675" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
     <clientData/>
   </oneCellAnchor>
 </wsDr>
@@ -1057,6 +1099,16 @@
           <t>Vaishnavi</t>
         </is>
       </c>
+      <c r="F7" s="7" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2025-05-04 08:29:11</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1344,7 +1396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1379,7 +1431,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1412,7 +1464,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>3.0</t>
         </is>
       </c>
     </row>
@@ -1424,7 +1476,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Anmol</t>
+          <t>Vaishnavi</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1488,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 08:27:31</t>
+          <t>2025-05-04 08:29:11</t>
         </is>
       </c>
     </row>
@@ -1448,7 +1500,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>[█-------------------] 7%</t>
+          <t>[███-----------------] 15%</t>
         </is>
       </c>
     </row>
@@ -1471,7 +1523,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1494,6 +1546,112 @@
       </c>
       <c r="B40" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Vaishnavi</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Task 3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Home &gt; Dashboard</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>Vaishnavi</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>2025-05-04 08:29:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="100" customHeight="1"/>
+    <row r="20">
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B20" s="8" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>fail</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update by Paul on Task 4.0
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Task ID 1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Task ID 3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Task ID 4" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -36,7 +37,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -59,6 +60,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FF6347"/>
         <bgColor rgb="00FF6347"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFB6C1"/>
+        <bgColor rgb="00FFB6C1"/>
       </patternFill>
     </fill>
   </fills>
@@ -89,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -103,6 +110,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,12 +398,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Summary'!$A$40:$A$41</f>
+              <f>'Summary'!$A$40:$A$42</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Summary'!$B$40:$B$41</f>
+              <f>'Summary'!$B$40:$B$42</f>
             </numRef>
           </val>
         </ser>
@@ -578,6 +587,39 @@
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400675" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2962275" cy="3810000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1209,6 +1251,16 @@
           <t>Paul</t>
         </is>
       </c>
+      <c r="F11" s="9" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-05-04 08:30:23</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1396,7 +1448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1441,7 +1493,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1464,7 +1516,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.0</t>
         </is>
       </c>
     </row>
@@ -1476,7 +1528,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Vaishnavi</t>
+          <t>Paul</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1540,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 08:29:11</t>
+          <t>2025-05-04 08:30:23</t>
         </is>
       </c>
     </row>
@@ -1500,7 +1552,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>[███-----------------] 15%</t>
+          <t>[████----------------] 23%</t>
         </is>
       </c>
     </row>
@@ -1523,7 +1575,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1555,6 +1607,16 @@
         </is>
       </c>
       <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1658,4 +1720,100 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Task 4.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>No Navigation</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>2025-05-04 08:30:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="100" customHeight="1"/>
+    <row r="20">
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>hold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update by Anmol on Task 1.1
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -503,6 +503,31 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>26</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5715000" cy="3219450"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -633,6 +658,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1041,6 +1069,16 @@
           <t>Anmol</t>
         </is>
       </c>
+      <c r="F3" s="9" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-05-04 08:31:05</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1352,7 +1390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1412,6 +1450,20 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
@@ -1433,6 +1485,79 @@
       <c r="B21" s="4" t="inlineStr">
         <is>
           <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>Task 1.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>Home &gt; Login &gt; Username</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>Anmol</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>2025-05-04 08:31:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="100" customHeight="1"/>
+    <row r="42">
+      <c r="A42" s="4" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B42" s="10" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>
@@ -1493,7 +1618,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -1516,7 +1641,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>1.1</t>
         </is>
       </c>
     </row>
@@ -1528,7 +1653,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Anmol</t>
         </is>
       </c>
     </row>
@@ -1540,7 +1665,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 08:30:23</t>
+          <t>2025-05-04 08:31:05</t>
         </is>
       </c>
     </row>
@@ -1552,7 +1677,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>[████----------------] 23%</t>
+          <t>[██████--------------] 30%</t>
         </is>
       </c>
     </row>
@@ -1575,7 +1700,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -1597,7 +1722,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">

</xml_diff>

<commit_message>
Update by Anmol on Task 1.2
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -524,6 +524,34 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>48</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="4552950" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1104,6 +1132,16 @@
           <t>Anmol</t>
         </is>
       </c>
+      <c r="F4" s="7" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-05-04 08:31:52</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1390,7 +1428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1488,6 +1526,7 @@
         </is>
       </c>
     </row>
+    <row r="22"/>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
@@ -1537,6 +1576,20 @@
       </c>
     </row>
     <row r="27" ht="100" customHeight="1"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
         <is>
@@ -1558,6 +1611,79 @@
       <c r="B43" s="4" t="inlineStr">
         <is>
           <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B45" s="4" t="inlineStr">
+        <is>
+          <t>Task 1.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B46" s="4" t="inlineStr">
+        <is>
+          <t>Home &gt; Login &gt; Password</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B47" s="4" t="inlineStr">
+        <is>
+          <t>Anmol</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B48" s="4" t="inlineStr">
+        <is>
+          <t>2025-05-04 08:31:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" ht="100" customHeight="1"/>
+    <row r="64">
+      <c r="A64" s="4" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B64" s="8" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B65" s="4" t="inlineStr">
+        <is>
+          <t>yep</t>
         </is>
       </c>
     </row>
@@ -1608,7 +1734,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -1641,7 +1767,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.1</t>
+          <t>1.2</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1791,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 08:31:05</t>
+          <t>2025-05-04 08:31:52</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1803,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>[██████--------------] 30%</t>
+          <t>[███████-------------] 38%</t>
         </is>
       </c>
     </row>
@@ -1700,7 +1826,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
@@ -1722,7 +1848,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">

</xml_diff>

<commit_message>
Update by Vaishnavi on Task 3.1
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -552,6 +552,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -656,6 +659,31 @@
         <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>26</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2543175" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1252,6 +1280,16 @@
           <t>Vaishnavi</t>
         </is>
       </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025-05-04 08:34:51</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1488,20 +1526,6 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
@@ -1526,7 +1550,6 @@
         </is>
       </c>
     </row>
-    <row r="22"/>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
@@ -1576,20 +1599,6 @@
       </c>
     </row>
     <row r="27" ht="100" customHeight="1"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
         <is>
@@ -1724,7 +1733,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -1755,7 +1764,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7.69%</t>
+          <t>15.38%</t>
         </is>
       </c>
     </row>
@@ -1767,7 +1776,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>3.1</t>
         </is>
       </c>
     </row>
@@ -1779,7 +1788,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Anmol</t>
+          <t>Vaishnavi</t>
         </is>
       </c>
     </row>
@@ -1791,7 +1800,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 08:31:52</t>
+          <t>2025-05-04 08:34:51</t>
         </is>
       </c>
     </row>
@@ -1803,7 +1812,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>[███████-------------] 38%</t>
+          <t>[█████████-----------] 46%</t>
         </is>
       </c>
     </row>
@@ -1826,7 +1835,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39">
@@ -1858,7 +1867,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
@@ -1883,7 +1892,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1943,6 +1952,20 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
@@ -1964,6 +1987,79 @@
       <c r="B21" s="4" t="inlineStr">
         <is>
           <t>fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>Task 3.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>Home &gt; Dashboard</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>Vaishnavi</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>2025-05-04 08:34:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="100" customHeight="1"/>
+    <row r="42">
+      <c r="A42" s="4" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B42" s="5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>Passed</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update by John on Task 5.0
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Task ID 3" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Task ID 4" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Task ID 2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Task ID 5" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -97,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -113,6 +114,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,12 +403,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Summary'!$A$40:$A$43</f>
+              <f>'Summary'!$A$40:$A$44</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Summary'!$B$40:$B$43</f>
+              <f>'Summary'!$B$40:$B$44</f>
             </numRef>
           </val>
         </ser>
@@ -751,6 +755,39 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5715000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1469,8 +1506,16 @@
           <t>John</t>
         </is>
       </c>
-      <c r="F13" s="2" t="n"/>
-      <c r="G13" s="2" t="n"/>
+      <c r="F13" s="11" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>2025-05-04 11:13:52</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1752,7 +1797,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1777,7 +1822,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -1808,7 +1853,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15.38%</t>
+          <t>23.08%</t>
         </is>
       </c>
     </row>
@@ -1820,7 +1865,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
@@ -1832,7 +1877,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Yash</t>
+          <t>John</t>
         </is>
       </c>
     </row>
@@ -1844,7 +1889,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 08:51:32</t>
+          <t>2025-05-04 11:13:52</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1901,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>[██████████----------] 53%</t>
+          <t>[████████████--------] 61%</t>
         </is>
       </c>
     </row>
@@ -1879,7 +1924,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
@@ -1931,6 +1976,16 @@
         </is>
       </c>
       <c r="B43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2299,4 +2354,100 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Task 5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Home &gt; Help &gt; FAQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>2025-05-04 11:13:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="100" customHeight="1"/>
+    <row r="20">
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>trst</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update by John on Task 5.1
</commit_message>
<xml_diff>
--- a/main_excel.xlsx
+++ b/main_excel.xlsx
@@ -788,6 +788,34 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>26</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5715000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1541,8 +1569,16 @@
           <t>John</t>
         </is>
       </c>
-      <c r="F14" s="2" t="n"/>
-      <c r="G14" s="2" t="n"/>
+      <c r="F14" s="11" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>2025-05-04 16:52:19</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1822,7 +1858,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -1853,7 +1889,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>23.08%</t>
+          <t>30.77%</t>
         </is>
       </c>
     </row>
@@ -1865,7 +1901,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>5.1</t>
         </is>
       </c>
     </row>
@@ -1889,7 +1925,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-04 11:13:52</t>
+          <t>2025-05-04 16:52:19</t>
         </is>
       </c>
     </row>
@@ -1901,7 +1937,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>[████████████--------] 61%</t>
+          <t>[█████████████-------] 69%</t>
         </is>
       </c>
     </row>
@@ -1924,7 +1960,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
@@ -1962,17 +1998,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Yash</t>
+          <t>John</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Yash</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1982,7 +2018,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -2362,7 +2398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2422,6 +2458,20 @@
       </c>
     </row>
     <row r="5" ht="100" customHeight="1"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
@@ -2443,6 +2493,79 @@
       <c r="B21" s="4" t="inlineStr">
         <is>
           <t>trst</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>Subtask</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>Task 5.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t>Navigation</t>
+        </is>
+      </c>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>Settings &gt; Notifications &gt; Opt-In</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="inlineStr">
+        <is>
+          <t>Tester Name</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>2025-05-04 16:52:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="100" customHeight="1"/>
+    <row r="42">
+      <c r="A42" s="4" t="inlineStr">
+        <is>
+          <t>Test Result</t>
+        </is>
+      </c>
+      <c r="B42" s="5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>

</xml_diff>